<commit_message>
feat: add remote deployment scripts, new queries, checker rev005, and analysis reports
- Add remote_deploy/ with deploy.sh, run_eval.sh, serve_results.sh, fetch_results.py for remote server evaluation
- Add 13 new queries to query_pools.yaml (from external contributors), quality-pruned from 16 to 83 total
- Add checker rev005 with content_quality_advanced judge criteria
- Add evaluation analysis reports and model comparison statistics
- Update checker_execute.py and checker_score.py with enhanced scoring logic
- Update batch_recheck.sh with incremental recheck support
</commit_message>
<xml_diff>
--- a/docs/人工构造数据时使用的prompt示例.xlsx
+++ b/docs/人工构造数据时使用的prompt示例.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feixiaoxu01/Documents/agents/agent_auto_evaluation/universal_scenario_framework/tmp_scenarios/novel_writing_alchemist/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4BBE07-5997-A345-A9F2-108A62AEC869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>模型交互记录</t>
   </si>
@@ -20,128 +28,7 @@
     <t>交互思路</t>
   </si>
   <si>
-    <t xml:space="preserve">user：
-请你帮我把下面这段内容调整功能为更自然、更符合一般用户习惯的表达。你可以对语句表达方式和结构顺序等内容做出修改，但禁止改动原内容中内涵的真实需求。以下是待修改的内容：
-“你是一名拥有 6 年以上内容视频脚本创作经验的内容视频脚本撰写专家，长期为小红书输出知识型、解释型内容视频脚本，深度理解小红书用户的内容偏好：
-重逻辑、重可信度、重解释清晰度，反感情绪化煽动与阴谋论式表达，偏好“把复杂问题讲明白”的内容风格。
-你熟悉小红书平台对社会心理与社会清晰等议题的内容边界与表达方式，擅长将抽象、容易被误解的概念，转译为理性、中立、可理解、可拍摄的内容视频脚本，在保证信息准确与合规的前提下，提高用户的认知获得感与完播率。
-任务说明
-请生成一条用于小红书发布的内容视频完整脚本，主题为：
-「你也线上确诊了？ADHD到底是怎么火起来的？」
-脚本要求：
-* 视频形式：口播 + 简单画面辅助
-* 视频总时长：3–4 分钟
-* 拍摄条件：单人出镜，室内拍摄，低成本可执行
-* 内容定位：知识解释型 / 概念澄清型
-* 目标效果：
-    * 帮助普通用户理解“ADHD”这一概念的真实含义
-    * 区分热梗与真实病症
-    * 避免制造恐慌或刻板印象，引导正确对待与正确就医。
-* 内容逻辑需清晰、循序渐进，适合小红书用户边看边理解的观看习惯。
-创作思路与方法约束
-* 开头需在 前 5 秒明确抛出问题或认知冲突，引导用户继续观看
-* 不使用阴谋论、情绪化判断或煽动性措辞
-* 所有观点需以解释、界定、澄清为核心，而非立场输出
-* 抽象概念必须转译为可拍的画面与行为（如：板书、手势指代、画面提示）
-* 节奏偏稳，但需通过分段结构与画面变化维持注意力
-* 明确哪些是公开信息层面的概念解释，避免给出具体作战细节或敏感推演
-禁止内容
-* 不得涉及任何形式的人身攻击
-* 不得引导仇恨、恐慌或极端情绪
-* 不得使用未经证实的内部消息、阴谋论式推断
-* 不得将内容写成病理分析、论文或纯观点输出
-* 不得忽略视频脚本属性，仅给解释性段落文本
-输出内容与格式要求
-请按以下结构输出，不得增减模块：
-一、视频基础设定
-* 视频主题
-* 表达形式
-* 目标平台与时长
-* 拍摄与制作说明
-二、内容结构概览
-* 开头吸引段：功能说明
-* 核心解释段：分段说明
-* 澄清与边界段：功能说明
-* 结尾收束段：功能说明
-三、完整内容视频脚本（按分镜输出）
-请按分镜顺序逐段输出，每一分镜单独成块，并统一使用以下格式：
-【分镜x】
-画面 / 镜头描述（景别、构图、是否推进/切换）
-布景 / 环境说明
-人物动作 / 肢体表现
-口播文案（口语化但不随意）
-音效 / 节奏提示（如无可写“无”）
-语言与专业要求
-* 全程保持理性、中立、解释型语气
-* 使用小红书用户可理解的表达，但不降低概念准确性
-* 合理使用专业词汇（如：等），避免术语堆砌
-* 表述需清晰区分：事实 / 解读 / 推测边界”
-bot：
-这份修改建议旨在将原本充满“指令代码感”的提示词，转化为更像是在**给一位专业合作伙伴下达 Brief（需求简报）**的沟通口吻。
-调整后的内容逻辑更顺畅（背景设定 -&gt; 核心任务 -&gt; 创作细节 -&gt; 输出格式），减少了机械的重复强调，但完全保留了你对**专业度、理性风格、合规性以及特定格式**的硬性要求。
-以下是调整后的提示词：
-***
-**【指令：小红书知识科普视频脚本创作】**
-**1. 角色设定与风格基调**
-请你扮演一位拥有 6 年经验的**知识型视频脚本专家**，专门为小红书用户创作深度且清晰的内容。
-你的强项是“把复杂问题讲明白”，风格要**理性、中立、重逻辑**，坚决摒弃情绪化煽动、阴谋论或毫无根据的焦虑制造。你需要将抽象的概念转化为用户听得懂的语言，并设计出低成本、可执行的画面动作（如手势、板书）。
-**2. 核心任务**
-请为我撰写一条时长约 **3–4 分钟**的口播视频脚本（单人出镜 + 简单画面辅助）。
-**视频主题：**「你也线上确诊了？ADHD 到底是怎么火起来的？」
-**核心目的：**
-*   **科普真相：** 帮助普通人理解 ADHD（注意缺陷与多动障碍）的医学真意。
-*   **澄清误区：** 区分网络热梗（如“这就是我”）与真实病症的区别。
-*   **正向引导：** 破除刻板印象，不制造恐慌，引导用户科学看待和正确就医。
-**3. 创作要求与注意事项**
-*   **开头策略：** 前 5 秒必须抛出认知冲突或核心痛点，留住用户。
-*   **内容逻辑：** 循序渐进，像剥洋葱一样层层深入，既要有专业词汇的支撑，又要用大白话解释清楚。
-*   **画面感：** 脚本不能只是“念稿子”，必须注明具体的画面表现（动作、神态、后期文字/图片提示），要让概念“看得见”。
-*   **红线规避：** 严禁人身攻击、严禁引用未经证实的“内部消息”或阴谋论。所有观点必须以客观事实和医学共识为基础，不要写成枯燥的论文，也不要写成情绪发泄。
-**4. 输出格式要求（请严格遵守）**
-请按照以下三个模块的顺序输出，不要遗漏：
-**第一部分：视频基础设定**
-（包含：视频主题、表达形式、目标平台与时长、拍摄与制作说明）
-**第二部分：内容结构概览**
-（请简要梳理：开头吸引段、核心解释段、澄清与边界段、结尾收束段 的功能逻辑）
-**第三部分：完整分镜脚本**
-请按分镜顺序逐段撰写，每一分镜作为一个独立模块，统一使用下方格式：
-&gt; **【分镜 X】**
-&gt; *   **画面 / 镜头描述：**（景别、构图、推拉运镜等）
-&gt; *   **布景 / 环境说明：**
-&gt; *   **人物动作 / 肢体表现：**
-&gt; *   **口播文案：**（要求口语化、自然，但逻辑严密）
-&gt; *   **音效 / 节奏提示：**（如无特殊设计可填“无”）
-***
-**修改思路说明（供参考）：**
-1.  **语气软化：** 将“你是一名……”改为“请你扮演……”，将生硬的“禁止内容”融入到“创作要求”中，读起来更像人与人的沟通。
-2.  **逻辑重组：** 原文中“创作思路”和“禁止内容”有部分重叠，调整后归纳为“风格基调”和“注意事项”，阅读更流畅。
-3.  **保留核心：** 你最看重的“理性中立”、“分镜格式”、“3-4分钟时长”等关键约束条件完全保留，未做任何删减。
-user：
-不要用结构化的形式，用段落式文本
-bot：
-好的，这是完全去除列表结构、采用纯段落式文本表达的指令版本。这样的表达方式就像你在给一位专业编导发一段详细的微信语音或邮件需求，既自然又保留了所有关键约束：
-***
-请你扮演一位拥有 6 年以上经验的资深内容视频脚本专家，你的专长是为小红书用户创作重逻辑、解释清晰且高度可信的知识型内容。你需要帮我策划并撰写一条主题为「你也线上确诊了？ADHD 到底是怎么火起来的？」的视频脚本。由于你的受众偏好“把复杂问题讲明白”且反感煽动情绪，所以请保持理性中立的基调，熟悉社会心理议题的边界，把抽象概念转化为容易理解且低成本可拍摄的画面（比如配合板书或特定手势），在不制造恐慌和阴谋论的前提下，引导大家区分网络热梗与真实病症，建立正确的就医认知。
-具体的创作要求是：视频采用单人出镜口播配合简单画面的形式，时长控制在 3 到 4 分钟。脚本开头的前 5 秒必须抛出有力的问题或认知冲突来留住用户；中间的内容逻辑要循序渐进，像剥洋葱一样把概念讲透，不要堆砌术语，也不要写成枯燥的论文或没有实操性的纯观点，所有抽象内容都要有对应的画面描述；结尾要收束有力。绝对禁止使用人身攻击、内部消息式推断或引导极端情绪的措辞，必须严格区分事实与解读的边界。
-最后，请务必按照以下顺序和格式输出内容，不要随意增减模块。第一部分先列出“视频基础设定”，包含主题、表达形式、平台时长和制作说明；第二部分给出“内容结构概览”，简要梳理开头、核心解释、澄清与边界、结尾这四段的功能；第三部分请输出按分镜划分的“完整视频脚本”。在第三部分中，每一个分镜都要单独成块，统一以【分镜 X】开头，紧接着依次写明画面描述（包含景别构图等）、布景环境说明、人物动作表现、口语化的口播文案，以及音效节奏提示。
-最终使用的prompt：
-你是一位拥有多年经验的知识型视频脚本专家，专门为小红书用户创作深度且清晰的内容。你的强项是“把复杂问题讲明白”，风格要理性、中立、重逻辑，拒绝情绪化煽动、阴谋论，或是毫无根据的制造焦虑。你需要将抽象的概念转化为用户听得懂的语言，并设计出低成本、可执行的画面动作（如手势、板书）。你还掌握生成脚本所必备的医学专业知识。
-现在请你为我撰写一条标题为“你也线上确诊了？ADHD 到底是怎么火起来的？”的口播视频脚本，时长大概约3–4分钟，我单人出镜，可以有简单的画面和动作辅助。视频主要输出三点内容：一是帮助普通人理解 ADHD（注意缺陷与多动障碍）的医学真相。二是区分网友玩梗时的确诊表现与真实病症的区别，澄清误区。三是正向引导观众，破除刻板印象，不制造恐慌，引导用户科学看待和正确就医。
-请按照以下三个模块的顺序输出，不要遗漏：
-第一部分：视频基础设定（包含：视频主题、表达形式、目标平台与时长、拍摄与制作说明）
-第二部分：内容结构（请简要梳理：开头吸引段、核心解释段、澄清与边界段、结尾收束段 的功能逻辑）
-第三部分：完整分镜脚本
-请按分镜顺序逐段撰写，每一分镜作为一个独立模块，统一使用下方格式：
-&gt; **【分镜 X】**
-&gt; *   **画面 / 镜头描述：**（景别、构图、推拉运镜等）
-&gt; *   **布景 / 环境说明：**
-&gt; *   **人物动作 / 肢体表现：**
-&gt; *   **口播文案：**（要求口语化、自然，但逻辑严密）
-&gt; *   **音效 / 节奏提示：**（如无特殊设计可填“无”）
-注意，你的开头前 5 秒必须抛出认知冲突或核心痛点，留住用户。后面的内容要循序渐进，层层深入，用大白话把专业知识解释清楚。你的所有观点必须以客观事实和医学共识为基础，严禁人身攻击，但也不能写成写成枯燥的论文，要有吸引看下去的点或爆点，但不能单纯是情绪发泄。注意你的脚本不应该只是念稿子，必须标注具体的动作、神态、后期文字/图片提示等画面表现。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">主要素材：1. 想好的主题/视频标题。2. 规范文档中的示例prompt。
+    <t>主要素材：1. 想好的主题/视频标题。2. 规范文档中的示例prompt。
 构造的主要思路是，以示例prompt为底本（保证完整、高质），利用模型将示例prompt的内容修改成符合主题、内部逻辑通顺的结构化prompt，之后人工进行细节调整，使其满足多样化要求。
 以下是具体步骤：
 首先，想好视频的主题（参考知乎/小红书的热榜）。
@@ -154,7 +41,7 @@
 3. 需要给出明确的格式示例，这里最好是结构化的，用自然语言很难给模型说明白。</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 我是一个b站生活区up主，下一期视频没灵感了，给我列一些选题看看，每条大致说说就行不用长篇大论展开讲
 &lt; ### bot &gt;：
 B站生活区（尤其是现在的环境）很看重**“人设”**、**“真实感”**或者**“反差”**。既然你没灵感，我就按拍摄难度和题材类型给你分几类，挑你觉得执行起来最顺手的：
@@ -437,14 +324,14 @@
 *   复刻过程中要体现出“看似简单，实则很多坑”的真实感。</t>
   </si>
   <si>
-    <t xml:space="preserve">1、没有思路，让模型给一些参考方向
+    <t>1、没有思路，让模型给一些参考方向
 2、从中挑选一个，再让模型生成prompt
 3、针对不满意的地方提出修改要求
 4、还是改不好，为避免前轮影响，新开一个对话重新问
 5、对大体可用的prompt手动调优直至满意</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 Role：
 你是一位业内顶尖的漫剧编剧大神，拥有丰富的IP改编与原创经验。你曾主笔过30部爆款漫剧脚本，题材涵盖职场逆袭、校园甜宠、仙侠玄幻、穿越重生等热门赛道。你深谙竖屏时代的视听语言，擅长将文字转化为极具画面感和冲击力的脚本。
 Goals：
@@ -605,7 +492,7 @@
 等我发你《甄嬛传》原著片段，你就按上面这些要求帮我改成漫剧剧本，可以吗？</t>
   </si>
   <si>
-    <t xml:space="preserve">思路：
+    <t>思路：
 1. 确定创作类型。
 2. 将规范中给的优质prompt示例发给模型，作为仿写的参考。
 3. 规定视频内容的主题或需要进行改编的小说，告诉模型按照该主题/小说风格进行改写。这一步会尽量选取自己擅长或熟知的内容，这样对模型生成的内容是否准确会更有认知，不需要过多查证。
@@ -928,13 +815,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1、第一步给模型标准prompt示例模版，让模型进行仿写。
+    <t>1、第一步给模型标准prompt示例模版，让模型进行仿写。
 2、第二步根据模型仿写内容具体表现对内容进一步交互限定。
 3、第三步一直与模型交互、微调直到模型产出满意的合适的prompt。
 4、如果一直不满意就换一个模型或新开一个聊天框，如果有不错的但有瑕疵的，可以挑一个最好的自己手动微调。</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 帮我生成一个根据小说片段改编成漫剧剧本的prompt，我希望以《我在阴间当牛马》为标题，生成第一集的剧本，内容需要非常吸引人，小说片段用占位符代替。prompt需要包含：模型设定、任务描述（体裁、集数、每集时长）、主要的创作方法（如何理解原文/梗概的剧情，如何撰写符合漫剧节奏的剧情，如何将原文描写转化为剧本的视听语言，如何使剧情符合受众期待等）、约束条件（剧情、角色等方面）、输出内容要求（应当输出哪几部分）、输出格式要求（给出具体的格式模板）、禁止内容（避免模型输出不符合要求或违规的内容）。你生成的prompt需要层级结构明确、板块划分清晰、重点内容突出
 &lt; ### bot &gt;：
 下面给你一份**可直接复制使用的高质量 Prompt 模板**，结构清晰、层级分明、偏专业工业化表达，适合用于“根据小说片段改编为漫剧剧本”，并已内置标题《我在阴间当牛马》与第一集定位，同时保留小说片段占位符。
@@ -1330,142 +1217,13 @@
 “啥罚都有，关小黑屋，下油锅，反正有你受的。”鬼魂说得绘声绘色。</t>
   </si>
   <si>
-    <t xml:space="preserve">1. 选定体裁、主题、时长
+    <t>1. 选定体裁、主题、时长
 2. 加入规范中必备的限制
 3. 一般模型生成的内容都比较单薄，让他再丰富一些（可以给他标准中的示例进行学习）
 4. 微调内容及格式</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
-为我生成一个将现有的小说改编为抖音短剧的通用prompt，具体要求如下：
-首先明确模型身份（如“资深短剧编剧、爆款制造机、钩子大师”），并绑定抖音平台生态认知，体现对用户偏好与传播逻辑的精准把控，从而调用模型内部相关知识和语言风格，确保剧本专业且适配平台。要求保持风格专业统一，精准匹配短剧创作需求，并明确平台审美偏好，约束情感表达、台词风格等，确保剧本符合平台传播特点与用户喜好。
-接下来明确输出目标，例如“将提供的小说文本转化为指定集数与时长的短剧剧本”，以指导模型完成具体创作任务，确保输出符合需求。
-在prompt中必须设定改编约束，包括视觉化、快节奏、30秒钩子等改编要求，以符合短剧特点与观众喜好，防止创作偏离方向，保证剧本质量。要求制定贴合平台与专业制作的可落地标准，覆盖台词、剧情、钩子设计等要素，并全面涵盖从剧情拆解到视觉信息补充的完整流程，以指导模型按专业标准创作，保证剧本质量与完整性。
-输出示例中应采用标准剧本格式（场景标题、角色、动作、台词等），并确保排版清晰，以便输出内容符合行业规范，便于用户快速获取核心信息。
-在生成的prompt中预留小说文本、剧情梗概等创作素材的占位符，以方便我自由替换需要参考的文本。
-添加特定受众（如18-25岁女性）设定情绪导向，以调整剧本情绪浓度、台词倾向等，增强内容针对性与吸引力。
-在prompt中必须设定创作禁区，如“禁止使用旁白、禁止平淡开场”等剧情设计禁区，以避免常见创作偏差，保障剧本质量。同时设定内容禁区，包括但不限于“禁止侵权、禁止描绘血腥画面、禁止涉黄、禁止擦边、禁止涉及现实人物、禁止涉政”等。
-&lt; ### bot &gt;：
-&lt;&lt;抖音小说改编爆款短剧通用创作Prompt&gt;&gt;
-# 角色定位
-你是**资深抖音短剧编剧、爆款钩子制造师、短剧改编全流程专家**，深耕抖音短剧生态3年以上，精准掌握抖音15-60秒竖屏短剧传播算法、用户观看习惯与爆款逻辑，擅长将小说文本转化为适配平台推荐机制、高完播率、高追更率的短剧剧本，对18-25岁核心受众的审美偏好、情绪触点、台词接受度有深度把控，输出内容符合短剧行业拍摄落地标准与平台审核规范。
-# 输出目标
-将用户提供的小说素材，改编为**指定集数、单集15-60秒**的抖音竖屏短剧标准剧本，实现小说核心剧情的视觉化落地，每集具备强开篇钩子、快节奏冲突、高情绪共鸣、结尾留悬，适配抖音竖屏拍摄与传播需求。
-# 待改编素材占位符
-【基础素材】
-1. 小说原文：{{此处粘贴需改编的小说完整章节/核心片段}}
-2. 小说核心梗概：{{此处粘贴小说主线剧情、人物设定、核心冲突、名场面}}
-3. 定制参数：{{集数：X集 | 单集时长：15/30/60秒 | 短剧风格：甜宠/虐恋/爽文/复仇/玄幻等 | 主角人设补充 | 特殊改编要求}}
-# 目标受众与情绪导向
-目标受众：**18-25岁女性**
-情绪导向：贴合该群体偏好的甜宠心动、虐恋共情、爽文解压、复仇解气等核心情绪，强化女性向情感共鸣，放大情绪张力，弱化晦涩叙事与复杂支线，台词与剧情贴合年轻女性审美与表达习惯。
-# 核心改编约束
-1. **节奏与钩子约束**
-    - 单集严格控制在15-60秒，无任何冗余铺垫，每3-5秒输出一个关键信息点
-    - 0-3秒必须抛出**视觉/台词强钩子**，10秒内落地核心冲突，30秒完成小反转/伏笔埋设
-    - 每集结尾必须设置强悬念/反转钩子，引导用户点击下一集、关注账号
-2. **视觉化转化约束**
-    - 小说心理描写、环境叙述、背景交代**全部转化为竖屏镜头语言+角色动作细节**，无纯文字化叙事
-    - 标注关键镜头（特写/中景/全景/慢动作）、道具、场景构图，适配手机竖屏观看
-3. **台词与剧情约束**
-    - 台词口语化、短句式，单句台词不超过15字，核心情绪台词重复强化记忆点
-    - 保留小说核心主线、高光名场面，删减无效支线与冗余情节，每集聚焦1个核心冲突
-    - 人物行为贴合原著人设，剧情逻辑连贯，集与集之间形成强剧情勾连
-4. **落地性约束**
-    - 补充音效、BGM、转场提示，满足短剧拍摄、后期制作的直接落地需求
-# 创作禁区
-## 一、剧情设计禁区
-1. 禁止使用旁白、画外音进行叙事，所有信息通过角色动作、台词、镜头呈现
-2. 禁止平淡开场、无冲突慢节奏铺垫
-3. 禁止长篇大论台词、无意义水剧情、信息密度过低
-4. 禁止单集无钩子、无结尾悬念，无法引导追更
-5. 禁止剧情逻辑断裂、人物行为OOC（脱离原著人设）
-## 二、内容合规禁区
-1. 禁止侵权改编，仅基于用户提供的授权小说内容创作
-2. 禁止描绘血腥暴力、惊悚恐怖、低俗擦边、涉黄涉俗内容
-3. 禁止涉及政治敏感、宗教迷信、现实人物/真实事件映射
-4. 禁止违背公序良俗、传递不良价值观
-5. 禁止违反抖音平台内容审核规范与社区公约
-# 标准输出格式（行业规范）
-## 第X集 | 时长：XX秒 | 风格：XXX
-【场景】场景编号+室内/室外+具体场景（竖屏适配）
-【镜头】镜头类型+画面内容（竖屏构图）
-【角色】角色名称
-【动作】肢体动作、面部表情、道具使用细节
-【台词】短句式口语台词
-【音效/BGM】适配音效/背景音乐标注
-【钩子/伏笔】本集核心钩子+结尾留悬说明
-# 输出示例
-## 第1集 | 时长：30秒 | 风格：甜宠
-【场景】01 室内 总裁办公室（竖屏）
-【镜头】特写 男主骨节分明的手捏住女主递来的文件
-【角色】苏晚
-【动作】指尖微颤，抬头撞进男主视线，耳尖泛红
-【台词】总、总裁，文件……
-【角色】陆沉渊
-【动作】俯身逼近，气息压低，指尖轻刮女主耳尖
-【台词】叫我名字。
-【音效/BGM】心跳声+甜宠轻缓BGM
-【钩子/伏笔】男主突然的靠近打破距离感，结尾定格男主深邃眼神，留悬：他为何对自己格外特别？
-&lt; ### user &gt;：
-在“核心改编约束”的“视觉化转化约束”部分，将“心理描写、环境叙述、背景交代”等内容如何转化为竖屏镜头语言，写的详细一些，比如“用动作代替心理”等，不要举例。最后的“输出示例”删除。
-&lt; ### bot &gt;：
- 我将细化视觉化转化约束的具体方法，删除输出示例，同时保留prompt原有核心框架与专业性，贴合抖音短剧创作需求。
-# 抖音小说改编爆款短剧通用创作Prompt
-# 角色定位
-你是**资深抖音短剧编剧、爆款钩子制造师、短剧改编全流程专家**，深耕抖音短剧生态3年以上，精准掌握抖音15-60秒竖屏短剧传播算法、用户观看习惯与爆款逻辑，擅长将小说文本转化为适配平台推荐机制、高完播率、高追更率的短剧剧本，对18-25岁核心受众的审美偏好、情绪触点、台词接受度有深度把控，输出内容符合短剧行业拍摄落地标准与平台审核规范。
-# 输出目标
-将用户提供的小说素材，改编为**指定集数、单集15-60秒**的抖音竖屏短剧标准剧本，实现小说核心剧情的视觉化落地，每集具备强开篇钩子、快节奏冲突、高情绪共鸣、结尾留悬，适配抖音竖屏拍摄与传播需求。
-# 待改编素材占位符
-## 【基础素材】
-1. 小说原文：{{此处粘贴需改编的小说完整章节/核心片段}}
-2. 小说核心梗概：{{此处粘贴小说主线剧情、人物设定、核心冲突、名场面}}
-3. 定制参数：{{集数：X集 | 单集时长：15/30/60秒 | 短剧风格：甜宠/虐恋/爽文/复仇/玄幻等 | 主角人设补充 | 特殊改编要求}}
-# 目标受众与情绪导向
-目标受众：**18-25岁女性**
-情绪导向：贴合该群体偏好的甜宠心动、虐恋共情、爽文解压、复仇解气等核心情绪，强化女性向情感共鸣，放大情绪张力，弱化晦涩叙事与复杂支线，台词与剧情贴合年轻女性审美与表达习惯。
-# 核心改编约束
-## 1. 节奏与钩子约束
-- 单集严格控制在15-60秒，无任何冗余铺垫，每3-5秒输出一个关键信息点
-- 0-3秒必须抛出**视觉/台词强钩子**，10秒内落地核心冲突，30秒完成小反转/伏笔埋设
-- 每集结尾必须设置强悬念/反转钩子，引导用户点击下一集、关注账号
-## 2. 视觉化转化约束
-- 小说心理描写转化：以角色微表情、肢体动作、眼神变化替代直白心理表述，搭配适配的镜头运镜与光影变化强化情绪传递，贴合竖屏近距离呈现特点，让内心情绪可被直观感知，避免依赖文字解读；通过角色下意识动作、神态细节映射内心活动，凸显情绪张力，适配短剧快节奏情绪传递需求。
-- 小说环境叙述转化：结合竖屏构图特点，以局部特写、分层取景呈现环境细节，避免全景堆砌；用环境光影、道具摆放烘托剧情氛围，关联角色情绪，让环境成为剧情推进的辅助元素，同时适配手机竖屏观看的视觉聚焦需求，确保环境信息传递高效不冗余。
-- 小说背景交代转化：不单独设置铺垫段落，将背景信息融入角色动作、台词互动或道具细节中，通过碎片化呈现完成背景铺垫，贴合短剧快节奏叙事逻辑；优先筛选核心背景信息，剔除无关细节，确保背景交代不拖沓剧情，同时让观众快速理解故事前提，适配抖音用户碎片化观看习惯。
-- 整体视觉适配：所有镜头设计均贴合竖屏呈现，聚焦角色面部表情、手部动作等核心视觉点，避免画面信息杂乱；动作设计简洁有力、辨识度高，适配短剧拍摄落地，同时强化视觉冲击力，契合抖音平台用户对强视觉刺激的偏好。
-## 3. 台词与剧情约束
-- 台词口语化、短句式，单句台词不超过15字，核心情绪台词重复强化记忆点
-- 保留小说核心主线、高光名场面，删减无效支线与冗余情节，每集聚焦1个核心冲突
-- 人物行为贴合原著人设，剧情逻辑连贯，集与集之间形成强剧情勾连
-## 4. 落地性约束
-- 补充音效、BGM、转场提示，满足短剧拍摄、后期制作的直接落地需求
-# 创作禁区
-## 一、剧情设计禁区
-1. 禁止使用旁白、画外音进行叙事，所有信息通过角色动作、台词、镜头呈现
-2. 禁止平淡开场、无冲突慢节奏铺垫
-3. 禁止长篇大论台词、无意义水剧情、信息密度过低
-4. 禁止单集无钩子、无结尾悬念，无法引导追更
-5. 禁止剧情逻辑断裂、人物行为OOC（脱离原著人设）
-## 二、内容合规禁区
-1. 禁止侵权改编，仅基于用户提供的授权小说内容创作
-2. 禁止描绘血腥暴力、惊悚恐怖、低俗擦边、涉黄涉俗内容
-3. 禁止涉及政治敏感、宗教迷信、现实人物/真实事件映射
-4. 禁止违背公序良俗、传递不良价值观
-5. 禁止违反抖音平台内容审核规范与社区公约
-# 标准输出格式（行业规范）
-## 第X集 | 时长：XX秒 | 风格：XXX
-【场景】场景编号+室内/室外+具体场景（竖屏适配）
-【镜头】镜头类型+画面内容（竖屏构图）
-【角色】角色名称
-【动作】肢体动作、面部表情、道具使用细节
-【台词】短句式口语台词
-【音效/BGM】适配音效/背景音乐标注
-【钩子/伏笔】本集核心钩子+结尾留悬说明
-需要我帮你**适配特定短剧风格**（甜宠/爽文等）进一步优化约束细则吗？ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1、先整理规范中的优质prompt要求，并形成初始的要求列表
+    <t>1、先整理规范中的优质prompt要求，并形成初始的要求列表
 2、结合前一步整理的要求，让模型先生成一个初始的通用prompt
 3、多轮交互微调prompt中存在的问题与缺失
 4、多轮交互中删除prompt中存在预设小说内容的示例，以免使用prompt时模型生硬套用</t>
@@ -1556,7 +1314,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1.把规范中的漫剧剧本prompt示例稍微修改一下，增加场次/幕要求，并给出格式示例，然后让模型仿写复杂长query。
+    <t>1.把规范中的漫剧剧本prompt示例稍微修改一下，增加场次/幕要求，并给出格式示例，然后让模型仿写复杂长query。
 注意点：因为有时候只输出仿写prompt的指令，模型会直接输出答案，导致无效交互。所以一开始让模型仿写的时候，告诉模型不要直接输出答案，强调只要仿写结果，不输出其他额外信息。
 2.根据模型表现结果，给出下一步指令，因为第一步没有强调主题方向，模型给出了另一个体裁的prompt，所以第二轮query说明了还是需要漫剧剧本，让模型重新生成。
 3.模型重新生成结果良好，进行手动润色。
@@ -1564,7 +1322,7 @@
 修改人设技能：模型当前的第一个技能“视觉化表达能力”细节要求像是分镜表格的要求，但目前格式不要求表格，所以稍微修改了一下。</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 你是一个10年短剧行业资深编剧+大纲策划导师（擅长抖音/快手竖屏短剧，主导过30+爆款短剧大纲创作，深谙平台流量逻辑与落地拍摄需求。专业严谨且务实，善于拆解核心需求，语言直白不绕弯，能精准捕捉短剧“快节奏、强冲突、高情绪”核心，同时兼顾人设逻辑与传播性。
 核心任务
 为我生成抖音专属12集竖屏短剧（单集2分钟）大纲，严格适配下沉女性受众，核心基调为高燃复仇爽感。具体要求如下：
@@ -1827,7 +1585,7 @@
 （针对拍摄落地的建议，如：服化道风格、关键道具、场景氛围建议）</t>
   </si>
   <si>
-    <t xml:space="preserve">第一步：遴选较为优质prompt，美妆行业复仇爽剧提供了基础框架和核心要求，但缺少明确格式输出规范，准备借助模型重构仿写这个prompt。
+    <t>第一步：遴选较为优质prompt，美妆行业复仇爽剧提供了基础框架和核心要求，但缺少明确格式输出规范，准备借助模型重构仿写这个prompt。
 第二步：要求bot重构优质prompt，重点优化人物设定和情节框架，提升专业度。
 第三步：为提升prompt多样性，要求将背景从美妆行业改为律政行业，并更换人物姓名。
 第四步：由于上一轮答复给出了更多文案脚本大纲的内容，明确要求仿写prompt而非创作大纲，强调输出格式的完整性和结构性。
@@ -1835,7 +1593,7 @@
 第五步：由于上一轮前后引导语冗长，要求去除所有解释性内容，只保留简洁、可直接使用的完整prompt。最终得到结构清晰、指令明确的prompt。</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 我准备把一个小说改成漫剧。首先你要知道漫剧的创作需要经过从原始的抽象文本（小说、大纲等），到可视化、指令化的文本（剧本/脚本），再到具体的多媒体内容生成（图像、音频及最终的成品漫剧）的转化步骤。你要注意以下两点： 1. 生成的脚本需要承接原著小说（或其他素材）中的关键剧情、设定等“卖点”，将小说文本/原始创意按照合适的体量分集进行拆分，调整叙事节奏，使之符合短视频创作的需求。 2. 生成的脚本应负责剔除无效信息、补全视觉信息，把小说中模糊的意境（如“凄凉的月色”）和复杂的心理（如“他内心挣扎了很久”）翻译成可拍摄、可生成、可视化程度高的指令（如“少年站在月光下的枯树旁，低头看着颤抖的双拳”）。 需要你帮我构思一个完美的prompt，以便我之后用于生成小说改编的漫剧脚本。要详细，适合古风小说。prompt要结构化且完整，要包含人设、写作技法、每集时长、镜头数、输出格式要求等，同时要符合行业标准。生成出的prompt要能达到借由此prompt生成的脚本文本流畅、逻辑好，勾子多，吸引人。不要过于生硬follow我提出的这些要求，要有机地消化后生成一个不过于冗长又比较精细，方便直接生成脚本的prompt。
 &lt; ### bot &gt;：
 # 古风小说改编漫剧短视频脚本生成Prompt
@@ -2142,13 +1900,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">思路：
+    <t>思路：
 1. 先找一个较高质的prompt作为范例，输入“参照以下范例，生成新的prompt”等指令。为避免模型生成多余内容，可添加“不要输出其他额外信息，直接输出结果”。
 2. 若模型生成的prompt，不符合你的主题或体裁等要求，可添加修改指令，如“我还是想要分镜脚本，不要方案”。
 3. 若对模型生成的prompt不满意，可添加润色修改指令，如“调整语言表达和结构顺序等，但不要遗漏核心要素和真实需求。”</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 一条优质的爆款娱乐八卦内容视频需要具备哪些条件和特点
 &lt; ### bot &gt;：
 优质爆款娱乐八卦内容视频的必备条件与特点
@@ -2283,7 +2041,7 @@
 需要我帮你**精简脚本时长至20秒内**，同时保留爆款核心要素吗？</t>
   </si>
   <si>
-    <t xml:space="preserve">以娱乐八卦内容视频为例：
+    <t>以娱乐八卦内容视频为例：
 1. 可以先问模型：一条优质的爆款娱乐八卦内容视频需要具备哪些条件和特点，模型给了选题、内容、呈现、互动等方面的条件与特点，然后以这些方面作为构建prompt的各个板块，并根据模型给的条件进行下一步选的发问。
 2. 让模型给出近期比较有热度和话题度的一些娱乐事件，然后从中选出非常具有国民性和争议性、容易引起讨论的事件作为【视频选题】；
 3. 搜索几篇关于该事件的文章，最好包含不同角度的评价，保证信息量丰富，用这些文章作为【参考信息】；
@@ -2291,7 +2049,7 @@
 5. 让模型给出一个该垂类内容下的优质脚本，作为【输出示例】。</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; ### user &gt;：
+    <t>&lt; ### user &gt;：
 # 角色
 你是一位资深短剧编剧、爆款制造机和“钩子”大师。你深谙短剧观众的爽点，擅长通过紧凑的节奏和强烈的冲突留住观众。
 # 任务指令
@@ -2462,69 +2220,655 @@
 不需要整本小说。你只需要复制小说的**前3-5章**（通常是“黄金三章”），因为网文的开头就是为了留住读者，冲突最密集，最适合改编成短剧的第一集。</t>
   </si>
   <si>
-    <t xml:space="preserve">1. 先选择内容方向。2. 给模型一个这个方向的优质prompt让模型进行仿写，一般这一轮模型都会生成一个较为优质的答复。3. 询问模型适配这个prompt的素材有哪些。4. 参考模型意见和自己的经验选取素材。4. 最后将prompt和素材整合到一起。</t>
+    <t>1. 先选择内容方向。2. 给模型一个这个方向的优质prompt让模型进行仿写，一般这一轮模型都会生成一个较为优质的答复。3. 询问模型适配这个prompt的素材有哪些。4. 参考模型意见和自己的经验选取素材。4. 最后将prompt和素材整合到一起。</t>
+  </si>
+  <si>
+    <t>user：
+请你帮我把下面这段内容调整功能为更自然、更符合一般用户习惯的表达。你可以对语句表达方式和结构顺序等内容做出修改，但禁止改动原内容中内涵的真实需求。以下是待修改的内容：
+“你是一名拥有 6 年以上内容视频脚本创作经验的内容视频脚本撰写专家，长期为小红书输出知识型、解释型内容视频脚本，深度理解小红书用户的内容偏好：
+重逻辑、重可信度、重解释清晰度，反感情绪化煽动与阴谋论式表达，偏好“把复杂问题讲明白”的内容风格。
+你熟悉小红书平台对社会心理与社会清晰等议题的内容边界与表达方式，擅长将抽象、容易被误解的概念，转译为理性、中立、可理解、可拍摄的内容视频脚本，在保证信息准确与合规的前提下，提高用户的认知获得感与完播率。
+任务说明
+请生成一条用于小红书发布的内容视频完整脚本，主题为：
+「你也线上确诊了？ADHD到底是怎么火起来的？」
+脚本要求：
+* 视频形式：口播 + 简单画面辅助
+* 视频总时长：3–4 分钟
+* 拍摄条件：单人出镜，室内拍摄，低成本可执行
+* 内容定位：知识解释型 / 概念澄清型
+* 目标效果：
+    * 帮助普通用户理解“ADHD”这一概念的真实含义
+    * 区分热梗与真实病症
+    * 避免制造恐慌或刻板印象，引导正确对待与正确就医。
+* 内容逻辑需清晰、循序渐进，适合小红书用户边看边理解的观看习惯。
+创作思路与方法约束
+* 开头需在 前 5 秒明确抛出问题或认知冲突，引导用户继续观看
+* 不使用阴谋论、情绪化判断或煽动性措辞
+* 所有观点需以解释、界定、澄清为核心，而非立场输出
+* 抽象概念必须转译为可拍的画面与行为（如：板书、手势指代、画面提示）
+* 节奏偏稳，但需通过分段结构与画面变化维持注意力
+* 明确哪些是公开信息层面的概念解释，避免给出具体作战细节或敏感推演
+禁止内容
+* 不得涉及任何形式的人身攻击
+* 不得引导仇恨、恐慌或极端情绪
+* 不得使用未经证实的内部消息、阴谋论式推断
+* 不得将内容写成病理分析、论文或纯观点输出
+* 不得忽略视频脚本属性，仅给解释性段落文本
+输出内容与格式要求
+请按以下结构输出，不得增减模块：
+一、视频基础设定
+* 视频主题
+* 表达形式
+* 目标平台与时长
+* 拍摄与制作说明
+二、内容结构概览
+* 开头吸引段：功能说明
+* 核心解释段：分段说明
+* 澄清与边界段：功能说明
+* 结尾收束段：功能说明
+三、完整内容视频脚本（按分镜输出）
+请按分镜顺序逐段输出，每一分镜单独成块，并统一使用以下格式：
+【分镜x】
+画面 / 镜头描述（景别、构图、是否推进/切换）
+布景 / 环境说明
+人物动作 / 肢体表现
+口播文案（口语化但不随意）
+音效 / 节奏提示（如无可写“无”）
+语言与专业要求
+* 全程保持理性、中立、解释型语气
+* 使用小红书用户可理解的表达，但不降低概念准确性
+* 合理使用专业词汇（如：等），避免术语堆砌
+* 表述需清晰区分：事实 / 解读 / 推测边界”
+bot：
+这份修改建议旨在将原本充满“指令代码感”的提示词，转化为更像是在**给一位专业合作伙伴下达 Brief（需求简报）**的沟通口吻。
+调整后的内容逻辑更顺畅（背景设定 -&gt; 核心任务 -&gt; 创作细节 -&gt; 输出格式），减少了机械的重复强调，但完全保留了你对**专业度、理性风格、合规性以及特定格式**的硬性要求。
+以下是调整后的提示词：
+***
+**【指令：小红书知识科普视频脚本创作】**
+**1. 角色设定与风格基调**
+请你扮演一位拥有 6 年经验的**知识型视频脚本专家**，专门为小红书用户创作深度且清晰的内容。
+你的强项是“把复杂问题讲明白”，风格要**理性、中立、重逻辑**，坚决摒弃情绪化煽动、阴谋论或毫无根据的焦虑制造。你需要将抽象的概念转化为用户听得懂的语言，并设计出低成本、可执行的画面动作（如手势、板书）。
+**2. 核心任务**
+请为我撰写一条时长约 **3–4 分钟**的口播视频脚本（单人出镜 + 简单画面辅助）。
+**视频主题：**「你也线上确诊了？ADHD 到底是怎么火起来的？」
+**核心目的：**
+*   **科普真相：** 帮助普通人理解 ADHD（注意缺陷与多动障碍）的医学真意。
+*   **澄清误区：** 区分网络热梗（如“这就是我”）与真实病症的区别。
+*   **正向引导：** 破除刻板印象，不制造恐慌，引导用户科学看待和正确就医。
+**3. 创作要求与注意事项**
+*   **开头策略：** 前 5 秒必须抛出认知冲突或核心痛点，留住用户。
+*   **内容逻辑：** 循序渐进，像剥洋葱一样层层深入，既要有专业词汇的支撑，又要用大白话解释清楚。
+*   **画面感：** 脚本不能只是“念稿子”，必须注明具体的画面表现（动作、神态、后期文字/图片提示），要让概念“看得见”。
+*   **红线规避：** 严禁人身攻击、严禁引用未经证实的“内部消息”或阴谋论。所有观点必须以客观事实和医学共识为基础，不要写成枯燥的论文，也不要写成情绪发泄。
+**4. 输出格式要求（请严格遵守）**
+请按照以下三个模块的顺序输出，不要遗漏：
+**第一部分：视频基础设定**
+（包含：视频主题、表达形式、目标平台与时长、拍摄与制作说明）
+**第二部分：内容结构概览**
+（请简要梳理：开头吸引段、核心解释段、澄清与边界段、结尾收束段 的功能逻辑）
+**第三部分：完整分镜脚本**
+请按分镜顺序逐段撰写，每一分镜作为一个独立模块，统一使用下方格式：
+&gt; **【分镜 X】**
+&gt; *   **画面 / 镜头描述：**（景别、构图、推拉运镜等）
+&gt; *   **布景 / 环境说明：**
+&gt; *   **人物动作 / 肢体表现：**
+&gt; *   **口播文案：**（要求口语化、自然，但逻辑严密）
+&gt; *   **音效 / 节奏提示：**（如无特殊设计可填“无”）
+***
+**修改思路说明（供参考）：**
+1.  **语气软化：** 将“你是一名……”改为“请你扮演……”，将生硬的“禁止内容”融入到“创作要求”中，读起来更像人与人的沟通。
+2.  **逻辑重组：** 原文中“创作思路”和“禁止内容”有部分重叠，调整后归纳为“风格基调”和“注意事项”，阅读更流畅。
+3.  **保留核心：** 你最看重的“理性中立”、“分镜格式”、“3-4分钟时长”等关键约束条件完全保留，未做任何删减。
+user：
+不要用结构化的形式，用段落式文本
+bot：
+好的，这是完全去除列表结构、采用纯段落式文本表达的指令版本。这样的表达方式就像你在给一位专业编导发一段详细的微信语音或邮件需求，既自然又保留了所有关键约束：
+***
+请你扮演一位拥有 6 年以上经验的资深内容视频脚本专家，你的专长是为小红书用户创作重逻辑、解释清晰且高度可信的知识型内容。你需要帮我策划并撰写一条主题为「你也线上确诊了？ADHD 到底是怎么火起来的？」的视频脚本。由于你的受众偏好“把复杂问题讲明白”且反感煽动情绪，所以请保持理性中立的基调，熟悉社会心理议题的边界，把抽象概念转化为容易理解且低成本可拍摄的画面（比如配合板书或特定手势），在不制造恐慌和阴谋论的前提下，引导大家区分网络热梗与真实病症，建立正确的就医认知。
+具体的创作要求是：视频采用单人出镜口播配合简单画面的形式，时长控制在 3 到 4 分钟。脚本开头的前 5 秒必须抛出有力的问题或认知冲突来留住用户；中间的内容逻辑要循序渐进，像剥洋葱一样把概念讲透，不要堆砌术语，也不要写成枯燥的论文或没有实操性的纯观点，所有抽象内容都要有对应的画面描述；结尾要收束有力。绝对禁止使用人身攻击、内部消息式推断或引导极端情绪的措辞，必须严格区分事实与解读的边界。
+最后，请务必按照以下顺序和格式输出内容，不要随意增减模块。第一部分先列出“视频基础设定”，包含主题、表达形式、平台时长和制作说明；第二部分给出“内容结构概览”，简要梳理开头、核心解释、澄清与边界、结尾这四段的功能；第三部分请输出按分镜划分的“完整视频脚本”。在第三部分中，每一个分镜都要单独成块，统一以【分镜 X】开头，紧接着依次写明画面描述（包含景别构图等）、布景环境说明、人物动作表现、口语化的口播文案，以及音效节奏提示。
+最终使用的prompt：
+你是一位拥有多年经验的知识型视频脚本专家，专门为小红书用户创作深度且清晰的内容。你的强项是“把复杂问题讲明白”，风格要理性、中立、重逻辑，拒绝情绪化煽动、阴谋论，或是毫无根据的制造焦虑。你需要将抽象的概念转化为用户听得懂的语言，并设计出低成本、可执行的画面动作（如手势、板书）。你还掌握生成脚本所必备的医学专业知识。
+现在请你为我撰写一条标题为“你也线上确诊了？ADHD 到底是怎么火起来的？”的口播视频脚本，时长大概约3–4分钟，我单人出镜，可以有简单的画面和动作辅助。视频主要输出三点内容：一是帮助普通人理解 ADHD（注意缺陷与多动障碍）的医学真相。二是区分网友玩梗时的确诊表现与真实病症的区别，澄清误区。三是正向引导观众，破除刻板印象，不制造恐慌，引导用户科学看待和正确就医。
+请按照以下三个模块的顺序输出，不要遗漏：
+第一部分：视频基础设定（包含：视频主题、表达形式、目标平台与时长、拍摄与制作说明）
+第二部分：内容结构（请简要梳理：开头吸引段、核心解释段、澄清与边界段、结尾收束段 的功能逻辑）
+第三部分：完整分镜脚本
+请按分镜顺序逐段撰写，每一分镜作为一个独立模块，统一使用下方格式：
+&gt; **【分镜 X】**
+&gt; *   **画面 / 镜头描述：**（景别、构图、推拉运镜等）
+&gt; *   **布景 / 环境说明：**
+&gt; *   **人物动作 / 肢体表现：**
+&gt; *   **口播文案：**（要求口语化、自然，但逻辑严密）
+&gt; *   **音效 / 节奏提示：**（如无特殊设计可填“无”）
+注意，你的开头前 5 秒必须抛出认知冲突或核心痛点，留住用户。后面的内容要循序渐进，层层深入，用大白话把专业知识解释清楚。你的所有观点必须以客观事实和医学共识为基础，严禁人身攻击，但也不能写成写成枯燥的论文，要有吸引看下去的点或爆点，但不能单纯是情绪发泄。注意你的脚本不应该只是念稿子，必须标注具体的动作、神态、后期文字/图片提示等画面表现。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; ### user &gt;：
+为我生成一个将现有的小说改编为抖音短剧的通用prompt，具体要求如下：
+首先明确模型身份（如“资深短剧编剧、爆款制造机、钩子大师”），并绑定抖音平台生态认知，体现对用户偏好与传播逻辑的精准把控，从而调用模型内部相关知识和语言风格，确保剧本专业且适配平台。要求保持风格专业统一，精准匹配短剧创作需求，并明确平台审美偏好，约束情感表达、台词风格等，确保剧本符合平台传播特点与用户喜好。
+接下来明确输出目标，例如“将提供的小说文本转化为指定集数与时长的短剧剧本”，以指导模型完成具体创作任务，确保输出符合需求。
+在prompt中必须设定改编约束，包括视觉化、快节奏、30秒钩子等改编要求，以符合短剧特点与观众喜好，防止创作偏离方向，保证剧本质量。要求制定贴合平台与专业制作的可落地标准，覆盖台词、剧情、钩子设计等要素，并全面涵盖从剧情拆解到视觉信息补充的完整流程，以指导模型按专业标准创作，保证剧本质量与完整性。
+输出示例中应采用标准剧本格式（场景标题、角色、动作、台词等），并确保排版清晰，以便输出内容符合行业规范，便于用户快速获取核心信息。
+在生成的prompt中预留小说文本、剧情梗概等创作素材的占位符，以方便我自由替换需要参考的文本。
+添加特定受众（如18-25岁女性）设定情绪导向，以调整剧本情绪浓度、台词倾向等，增强内容针对性与吸引力。
+在prompt中必须设定创作禁区，如“禁止使用旁白、禁止平淡开场”等剧情设计禁区，以避免常见创作偏差，保障剧本质量。同时设定内容禁区，包括但不限于“禁止侵权、禁止描绘血腥画面、禁止涉黄、禁止擦边、禁止涉及现实人物、禁止涉政”等。
+&lt; ### bot &gt;：
+&lt;&lt;抖音小说改编爆款短剧通用创作Prompt&gt;&gt;
+# 角色定位
+你是**资深抖音短剧编剧、爆款钩子制造师、短剧改编全流程专家**，深耕抖音短剧生态3年以上，精准掌握抖音15-60秒竖屏短剧传播算法、用户观看习惯与爆款逻辑，擅长将小说文本转化为适配平台推荐机制、高完播率、高追更率的短剧剧本，对18-25岁核心受众的审美偏好、情绪触点、台词接受度有深度把控，输出内容符合短剧行业拍摄落地标准与平台审核规范。
+# 输出目标
+将用户提供的小说素材，改编为**指定集数、单集15-60秒**的抖音竖屏短剧标准剧本，实现小说核心剧情的视觉化落地，每集具备强开篇钩子、快节奏冲突、高情绪共鸣、结尾留悬，适配抖音竖屏拍摄与传播需求。
+# 待改编素材占位符
+【基础素材】
+1. 小说原文：{{此处粘贴需改编的小说完整章节/核心片段}}
+2. 小说核心梗概：{{此处粘贴小说主线剧情、人物设定、核心冲突、名场面}}
+3. 定制参数：{{集数：X集 | 单集时长：15/30/60秒 | 短剧风格：甜宠/虐恋/爽文/复仇/玄幻等 | 主角人设补充 | 特殊改编要求}}
+# 目标受众与情绪导向
+目标受众：**18-25岁女性**
+情绪导向：贴合该群体偏好的甜宠心动、虐恋共情、爽文解压、复仇解气等核心情绪，强化女性向情感共鸣，放大情绪张力，弱化晦涩叙事与复杂支线，台词与剧情贴合年轻女性审美与表达习惯。
+# 核心改编约束
+1. **节奏与钩子约束**
+    - 单集严格控制在15-60秒，无任何冗余铺垫，每3-5秒输出一个关键信息点
+    - 0-3秒必须抛出**视觉/台词强钩子**，10秒内落地核心冲突，30秒完成小反转/伏笔埋设
+    - 每集结尾必须设置强悬念/反转钩子，引导用户点击下一集、关注账号
+2. **视觉化转化约束**
+    - 小说心理描写、环境叙述、背景交代**全部转化为竖屏镜头语言+角色动作细节**，无纯文字化叙事
+    - 标注关键镜头（特写/中景/全景/慢动作）、道具、场景构图，适配手机竖屏观看
+3. **台词与剧情约束**
+    - 台词口语化、短句式，单句台词不超过15字，核心情绪台词重复强化记忆点
+    - 保留小说核心主线、高光名场面，删减无效支线与冗余情节，每集聚焦1个核心冲突
+    - 人物行为贴合原著人设，剧情逻辑连贯，集与集之间形成强剧情勾连
+4. **落地性约束**
+    - 补充音效、BGM、转场提示，满足短剧拍摄、后期制作的直接落地需求
+# 创作禁区
+## 一、剧情设计禁区
+1. 禁止使用旁白、画外音进行叙事，所有信息通过角色动作、台词、镜头呈现
+2. 禁止平淡开场、无冲突慢节奏铺垫
+3. 禁止长篇大论台词、无意义水剧情、信息密度过低
+4. 禁止单集无钩子、无结尾悬念，无法引导追更
+5. 禁止剧情逻辑断裂、人物行为OOC（脱离原著人设）
+## 二、内容合规禁区
+1. 禁止侵权改编，仅基于用户提供的授权小说内容创作
+2. 禁止描绘血腥暴力、惊悚恐怖、低俗擦边、涉黄涉俗内容
+3. 禁止涉及政治敏感、宗教迷信、现实人物/真实事件映射
+4. 禁止违背公序良俗、传递不良价值观
+5. 禁止违反抖音平台内容审核规范与社区公约
+# 标准输出格式（行业规范）
+## 第X集 | 时长：XX秒 | 风格：XXX
+【场景】场景编号+室内/室外+具体场景（竖屏适配）
+【镜头】镜头类型+画面内容（竖屏构图）
+【角色】角色名称
+【动作】肢体动作、面部表情、道具使用细节
+【台词】短句式口语台词
+【音效/BGM】适配音效/背景音乐标注
+【钩子/伏笔】本集核心钩子+结尾留悬说明
+# 输出示例
+## 第1集 | 时长：30秒 | 风格：甜宠
+【场景】01 室内 总裁办公室（竖屏）
+【镜头】特写 男主骨节分明的手捏住女主递来的文件
+【角色】苏晚
+【动作】指尖微颤，抬头撞进男主视线，耳尖泛红
+【台词】总、总裁，文件……
+【角色】陆沉渊
+【动作】俯身逼近，气息压低，指尖轻刮女主耳尖
+【台词】叫我名字。
+【音效/BGM】心跳声+甜宠轻缓BGM
+【钩子/伏笔】男主突然的靠近打破距离感，结尾定格男主深邃眼神，留悬：他为何对自己格外特别？
+&lt; ### user &gt;：
+在“核心改编约束”的“视觉化转化约束”部分，将“心理描写、环境叙述、背景交代”等内容如何转化为竖屏镜头语言，写的详细一些，比如“用动作代替心理”等，不要举例。最后的“输出示例”删除。
+&lt; ### bot &gt;：
+ 我将细化视觉化转化约束的具体方法，删除输出示例，同时保留prompt原有核心框架与专业性，贴合抖音短剧创作需求。
+# 抖音小说改编爆款短剧通用创作Prompt
+# 角色定位
+你是**资深抖音短剧编剧、爆款钩子制造师、短剧改编全流程专家**，深耕抖音短剧生态3年以上，精准掌握抖音15-60秒竖屏短剧传播算法、用户观看习惯与爆款逻辑，擅长将小说文本转化为适配平台推荐机制、高完播率、高追更率的短剧剧本，对18-25岁核心受众的审美偏好、情绪触点、台词接受度有深度把控，输出内容符合短剧行业拍摄落地标准与平台审核规范。
+# 输出目标
+将用户提供的小说素材，改编为**指定集数、单集15-60秒**的抖音竖屏短剧标准剧本，实现小说核心剧情的视觉化落地，每集具备强开篇钩子、快节奏冲突、高情绪共鸣、结尾留悬，适配抖音竖屏拍摄与传播需求。
+# 待改编素材占位符
+## 【基础素材】
+1. 小说原文：{{此处粘贴需改编的小说完整章节/核心片段}}
+2. 小说核心梗概：{{此处粘贴小说主线剧情、人物设定、核心冲突、名场面}}
+3. 定制参数：{{集数：X集 | 单集时长：15/30/60秒 | 短剧风格：甜宠/虐恋/爽文/复仇/玄幻等 | 主角人设补充 | 特殊改编要求}}
+# 目标受众与情绪导向
+目标受众：**18-25岁女性**
+情绪导向：贴合该群体偏好的甜宠心动、虐恋共情、爽文解压、复仇解气等核心情绪，强化女性向情感共鸣，放大情绪张力，弱化晦涩叙事与复杂支线，台词与剧情贴合年轻女性审美与表达习惯。
+# 核心改编约束
+## 1. 节奏与钩子约束
+- 单集严格控制在15-60秒，无任何冗余铺垫，每3-5秒输出一个关键信息点
+- 0-3秒必须抛出**视觉/台词强钩子**，10秒内落地核心冲突，30秒完成小反转/伏笔埋设
+- 每集结尾必须设置强悬念/反转钩子，引导用户点击下一集、关注账号
+## 2. 视觉化转化约束
+- 小说心理描写转化：以角色微表情、肢体动作、眼神变化替代直白心理表述，搭配适配的镜头运镜与光影变化强化情绪传递，贴合竖屏近距离呈现特点，让内心情绪可被直观感知，避免依赖文字解读；通过角色下意识动作、神态细节映射内心活动，凸显情绪张力，适配短剧快节奏情绪传递需求。
+- 小说环境叙述转化：结合竖屏构图特点，以局部特写、分层取景呈现环境细节，避免全景堆砌；用环境光影、道具摆放烘托剧情氛围，关联角色情绪，让环境成为剧情推进的辅助元素，同时适配手机竖屏观看的视觉聚焦需求，确保环境信息传递高效不冗余。
+- 小说背景交代转化：不单独设置铺垫段落，将背景信息融入角色动作、台词互动或道具细节中，通过碎片化呈现完成背景铺垫，贴合短剧快节奏叙事逻辑；优先筛选核心背景信息，剔除无关细节，确保背景交代不拖沓剧情，同时让观众快速理解故事前提，适配抖音用户碎片化观看习惯。
+- 整体视觉适配：所有镜头设计均贴合竖屏呈现，聚焦角色面部表情、手部动作等核心视觉点，避免画面信息杂乱；动作设计简洁有力、辨识度高，适配短剧拍摄落地，同时强化视觉冲击力，契合抖音平台用户对强视觉刺激的偏好。
+## 3. 台词与剧情约束
+- 台词口语化、短句式，单句台词不超过15字，核心情绪台词重复强化记忆点
+- 保留小说核心主线、高光名场面，删减无效支线与冗余情节，每集聚焦1个核心冲突
+- 人物行为贴合原著人设，剧情逻辑连贯，集与集之间形成强剧情勾连
+## 4. 落地性约束
+- 补充音效、BGM、转场提示，满足短剧拍摄、后期制作的直接落地需求
+# 创作禁区
+## 一、剧情设计禁区
+1. 禁止使用旁白、画外音进行叙事，所有信息通过角色动作、台词、镜头呈现
+2. 禁止平淡开场、无冲突慢节奏铺垫
+3. 禁止长篇大论台词、无意义水剧情、信息密度过低
+4. 禁止单集无钩子、无结尾悬念，无法引导追更
+5. 禁止剧情逻辑断裂、人物行为OOC（脱离原著人设）
+## 二、内容合规禁区
+1. 禁止侵权改编，仅基于用户提供的授权小说内容创作
+2. 禁止描绘血腥暴力、惊悚恐怖、低俗擦边、涉黄涉俗内容
+3. 禁止涉及政治敏感、宗教迷信、现实人物/真实事件映射
+4. 禁止违背公序良俗、传递不良价值观
+5. 禁止违反抖音平台内容审核规范与社区公约
+# 标准输出格式（行业规范）
+## 第X集 | 时长：XX秒 | 风格：XXX
+【场景】场景编号+室内/室外+具体场景（竖屏适配）
+【镜头】镜头类型+画面内容（竖屏构图）
+【角色】角色名称
+【动作】肢体动作、面部表情、道具使用细节
+【台词】短句式口语台词
+【音效/BGM】适配音效/背景音乐标注
+【钩子/伏笔】本集核心钩子+结尾留悬说明
+需要我帮你**适配特定短剧风格**（甜宠/爽文等）进一步优化约束细则吗？ </t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+  </cellStyleXfs>
   <cellXfs count="3">
-    <xf fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="0" zeroHeight="0" thickTop="0" thickBottom="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="16" width="60.05" customWidth="1"/>
+    <col min="1" max="16" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
@@ -2542,12 +2886,12 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:16" ht="409.6">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2564,12 +2908,12 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2586,12 +2930,12 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2608,12 +2952,12 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="409.6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2630,12 +2974,12 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="409.6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2652,12 +2996,12 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
+    <row r="7" spans="1:16" ht="409.6">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2674,12 +3018,12 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="409.6">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2696,12 +3040,12 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="409.6">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2718,12 +3062,12 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="409.6">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2740,12 +3084,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="409.6">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2762,12 +3106,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="409.6">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2784,12 +3128,12 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="409.6">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2806,7 +3150,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2824,7 +3168,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2842,7 +3186,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2860,7 +3204,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:16">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2878,7 +3222,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:16">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2896,7 +3240,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:16">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2914,7 +3258,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:16">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2932,7 +3276,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:16">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2950,7 +3294,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:16">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2968,7 +3312,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:16">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2986,7 +3330,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:16">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3004,7 +3348,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:16">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3022,7 +3366,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:16">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3040,7 +3384,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:16">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3058,7 +3402,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:16">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3076,7 +3420,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:16">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3094,7 +3438,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:16">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3112,7 +3456,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:16">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3130,7 +3474,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:16">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3148,7 +3492,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:16">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3166,7 +3510,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:16">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3184,7 +3528,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:16">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3202,7 +3546,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:16">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3220,7 +3564,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:16">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3238,7 +3582,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:16">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3256,7 +3600,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:16">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3274,7 +3618,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:16">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3292,7 +3636,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:16">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3310,7 +3654,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:16">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3328,7 +3672,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:16">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3346,7 +3690,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:16">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3364,7 +3708,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:16">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3382,7 +3726,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:16">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3400,7 +3744,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:16">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3418,7 +3762,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:16">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3436,7 +3780,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:16">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3454,7 +3798,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:16">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3472,7 +3816,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:16">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3490,7 +3834,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:16">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3508,7 +3852,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:16">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3526,7 +3870,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:16">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3544,7 +3888,7 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:16">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3562,7 +3906,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:16">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3580,7 +3924,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:16">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3598,7 +3942,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:16">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3616,7 +3960,7 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:16">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3634,7 +3978,7 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:16">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3652,7 +3996,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:16">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3670,7 +4014,7 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:16">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3688,7 +4032,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:16">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3706,7 +4050,7 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:16">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3724,7 +4068,7 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:16">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3742,7 +4086,7 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:16">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3760,7 +4104,7 @@
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:16">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3778,7 +4122,7 @@
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:16">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3796,7 +4140,7 @@
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:16">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3814,7 +4158,7 @@
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:16">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3832,7 +4176,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:16">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3850,7 +4194,7 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:16">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3868,7 +4212,7 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:16">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3886,7 +4230,7 @@
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:16">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3904,7 +4248,7 @@
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:16">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3922,7 +4266,7 @@
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:16">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3940,7 +4284,7 @@
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:16">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3958,7 +4302,7 @@
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:16">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3976,7 +4320,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:16">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3994,7 +4338,7 @@
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:16">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4012,7 +4356,7 @@
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:16">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4030,7 +4374,7 @@
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:16">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4048,7 +4392,7 @@
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:16">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4066,7 +4410,7 @@
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:16">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4084,7 +4428,7 @@
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:16">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4102,7 +4446,7 @@
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:16">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4120,7 +4464,7 @@
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:16">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4138,7 +4482,7 @@
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:16">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4156,7 +4500,7 @@
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:16">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4174,7 +4518,7 @@
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:16">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4192,7 +4536,7 @@
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:16">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4210,7 +4554,7 @@
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:16">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4228,7 +4572,7 @@
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:16">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -4246,7 +4590,7 @@
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:16">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -4264,7 +4608,7 @@
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:16">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -4282,7 +4626,7 @@
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:16">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4300,7 +4644,7 @@
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:16">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4318,7 +4662,7 @@
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:16">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4336,7 +4680,7 @@
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:16">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4354,7 +4698,7 @@
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:16">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4372,7 +4716,7 @@
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:16">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -4390,7 +4734,7 @@
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:16">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4408,7 +4752,7 @@
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:16">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4426,7 +4770,7 @@
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:16">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4444,7 +4788,7 @@
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:16">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -4462,7 +4806,7 @@
       <c r="O105" s="1"/>
       <c r="P105" s="1"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:16">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -4480,7 +4824,7 @@
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:16">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4498,7 +4842,7 @@
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:16">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -4516,7 +4860,7 @@
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:16">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -4534,7 +4878,7 @@
       <c r="O109" s="1"/>
       <c r="P109" s="1"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:16">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -4552,7 +4896,7 @@
       <c r="O110" s="1"/>
       <c r="P110" s="1"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:16">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -4570,7 +4914,7 @@
       <c r="O111" s="1"/>
       <c r="P111" s="1"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:16">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -4588,7 +4932,7 @@
       <c r="O112" s="1"/>
       <c r="P112" s="1"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:16">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -4606,7 +4950,7 @@
       <c r="O113" s="1"/>
       <c r="P113" s="1"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:16">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -4624,7 +4968,7 @@
       <c r="O114" s="1"/>
       <c r="P114" s="1"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:16">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -4642,7 +4986,7 @@
       <c r="O115" s="1"/>
       <c r="P115" s="1"/>
     </row>
-    <row r="116">
+    <row r="116" spans="1:16">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -4660,7 +5004,7 @@
       <c r="O116" s="1"/>
       <c r="P116" s="1"/>
     </row>
-    <row r="117">
+    <row r="117" spans="1:16">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -4678,7 +5022,7 @@
       <c r="O117" s="1"/>
       <c r="P117" s="1"/>
     </row>
-    <row r="118">
+    <row r="118" spans="1:16">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -4696,7 +5040,7 @@
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
     </row>
-    <row r="119">
+    <row r="119" spans="1:16">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -4714,7 +5058,7 @@
       <c r="O119" s="1"/>
       <c r="P119" s="1"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:16">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -4732,7 +5076,7 @@
       <c r="O120" s="1"/>
       <c r="P120" s="1"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:16">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -4750,7 +5094,7 @@
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
     </row>
-    <row r="122">
+    <row r="122" spans="1:16">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -4768,7 +5112,7 @@
       <c r="O122" s="1"/>
       <c r="P122" s="1"/>
     </row>
-    <row r="123">
+    <row r="123" spans="1:16">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -4786,7 +5130,7 @@
       <c r="O123" s="1"/>
       <c r="P123" s="1"/>
     </row>
-    <row r="124">
+    <row r="124" spans="1:16">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -4804,7 +5148,7 @@
       <c r="O124" s="1"/>
       <c r="P124" s="1"/>
     </row>
-    <row r="125">
+    <row r="125" spans="1:16">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -4822,7 +5166,7 @@
       <c r="O125" s="1"/>
       <c r="P125" s="1"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:16">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4840,7 +5184,7 @@
       <c r="O126" s="1"/>
       <c r="P126" s="1"/>
     </row>
-    <row r="127">
+    <row r="127" spans="1:16">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -4858,7 +5202,7 @@
       <c r="O127" s="1"/>
       <c r="P127" s="1"/>
     </row>
-    <row r="128">
+    <row r="128" spans="1:16">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -4876,7 +5220,7 @@
       <c r="O128" s="1"/>
       <c r="P128" s="1"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:16">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -4894,7 +5238,7 @@
       <c r="O129" s="1"/>
       <c r="P129" s="1"/>
     </row>
-    <row r="130">
+    <row r="130" spans="1:16">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -4912,7 +5256,7 @@
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
     </row>
-    <row r="131">
+    <row r="131" spans="1:16">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -4930,7 +5274,7 @@
       <c r="O131" s="1"/>
       <c r="P131" s="1"/>
     </row>
-    <row r="132">
+    <row r="132" spans="1:16">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -4948,7 +5292,7 @@
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
     </row>
-    <row r="133">
+    <row r="133" spans="1:16">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -4966,7 +5310,7 @@
       <c r="O133" s="1"/>
       <c r="P133" s="1"/>
     </row>
-    <row r="134">
+    <row r="134" spans="1:16">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -4984,7 +5328,7 @@
       <c r="O134" s="1"/>
       <c r="P134" s="1"/>
     </row>
-    <row r="135">
+    <row r="135" spans="1:16">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -5002,7 +5346,7 @@
       <c r="O135" s="1"/>
       <c r="P135" s="1"/>
     </row>
-    <row r="136">
+    <row r="136" spans="1:16">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -5020,7 +5364,7 @@
       <c r="O136" s="1"/>
       <c r="P136" s="1"/>
     </row>
-    <row r="137">
+    <row r="137" spans="1:16">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -5038,7 +5382,7 @@
       <c r="O137" s="1"/>
       <c r="P137" s="1"/>
     </row>
-    <row r="138">
+    <row r="138" spans="1:16">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -5056,7 +5400,7 @@
       <c r="O138" s="1"/>
       <c r="P138" s="1"/>
     </row>
-    <row r="139">
+    <row r="139" spans="1:16">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -5074,7 +5418,7 @@
       <c r="O139" s="1"/>
       <c r="P139" s="1"/>
     </row>
-    <row r="140">
+    <row r="140" spans="1:16">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -5092,7 +5436,7 @@
       <c r="O140" s="1"/>
       <c r="P140" s="1"/>
     </row>
-    <row r="141">
+    <row r="141" spans="1:16">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -5110,7 +5454,7 @@
       <c r="O141" s="1"/>
       <c r="P141" s="1"/>
     </row>
-    <row r="142">
+    <row r="142" spans="1:16">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -5128,7 +5472,7 @@
       <c r="O142" s="1"/>
       <c r="P142" s="1"/>
     </row>
-    <row r="143">
+    <row r="143" spans="1:16">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -5146,7 +5490,7 @@
       <c r="O143" s="1"/>
       <c r="P143" s="1"/>
     </row>
-    <row r="144">
+    <row r="144" spans="1:16">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -5164,7 +5508,7 @@
       <c r="O144" s="1"/>
       <c r="P144" s="1"/>
     </row>
-    <row r="145">
+    <row r="145" spans="1:16">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -5182,7 +5526,7 @@
       <c r="O145" s="1"/>
       <c r="P145" s="1"/>
     </row>
-    <row r="146">
+    <row r="146" spans="1:16">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -5200,7 +5544,7 @@
       <c r="O146" s="1"/>
       <c r="P146" s="1"/>
     </row>
-    <row r="147">
+    <row r="147" spans="1:16">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -5218,7 +5562,7 @@
       <c r="O147" s="1"/>
       <c r="P147" s="1"/>
     </row>
-    <row r="148">
+    <row r="148" spans="1:16">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -5236,7 +5580,7 @@
       <c r="O148" s="1"/>
       <c r="P148" s="1"/>
     </row>
-    <row r="149">
+    <row r="149" spans="1:16">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -5254,7 +5598,7 @@
       <c r="O149" s="1"/>
       <c r="P149" s="1"/>
     </row>
-    <row r="150">
+    <row r="150" spans="1:16">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -5272,7 +5616,7 @@
       <c r="O150" s="1"/>
       <c r="P150" s="1"/>
     </row>
-    <row r="151">
+    <row r="151" spans="1:16">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -5290,7 +5634,7 @@
       <c r="O151" s="1"/>
       <c r="P151" s="1"/>
     </row>
-    <row r="152">
+    <row r="152" spans="1:16">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -5308,7 +5652,7 @@
       <c r="O152" s="1"/>
       <c r="P152" s="1"/>
     </row>
-    <row r="153">
+    <row r="153" spans="1:16">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -5326,7 +5670,7 @@
       <c r="O153" s="1"/>
       <c r="P153" s="1"/>
     </row>
-    <row r="154">
+    <row r="154" spans="1:16">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -5344,7 +5688,7 @@
       <c r="O154" s="1"/>
       <c r="P154" s="1"/>
     </row>
-    <row r="155">
+    <row r="155" spans="1:16">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -5362,7 +5706,7 @@
       <c r="O155" s="1"/>
       <c r="P155" s="1"/>
     </row>
-    <row r="156">
+    <row r="156" spans="1:16">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -5380,7 +5724,7 @@
       <c r="O156" s="1"/>
       <c r="P156" s="1"/>
     </row>
-    <row r="157">
+    <row r="157" spans="1:16">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -5398,7 +5742,7 @@
       <c r="O157" s="1"/>
       <c r="P157" s="1"/>
     </row>
-    <row r="158">
+    <row r="158" spans="1:16">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -5416,43 +5760,44 @@
       <c r="O158" s="1"/>
       <c r="P158" s="1"/>
     </row>
-    <row r="159">
-      <c r="A159" s="2"/>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
-      <c r="F159" s="2"/>
-      <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
-      <c r="L159" s="2"/>
-      <c r="M159" s="2"/>
-      <c r="N159" s="2"/>
-      <c r="O159" s="2"/>
-      <c r="P159" s="2"/>
-    </row>
-    <row r="160">
-      <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
-      <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
-      <c r="L160" s="2"/>
-      <c r="M160" s="2"/>
-      <c r="N160" s="2"/>
-      <c r="O160" s="2"/>
-      <c r="P160" s="2"/>
+    <row r="159" spans="1:16">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+      <c r="O159" s="1"/>
+      <c r="P159" s="1"/>
+    </row>
+    <row r="160" spans="1:16">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+      <c r="O160" s="1"/>
+      <c r="P160" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>